<commit_message>
Add task 1 Update 3
</commit_message>
<xml_diff>
--- a/vacancy.xlsx
+++ b/vacancy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="131">
   <si>
     <t>name</t>
   </si>
@@ -37,69 +37,63 @@
     <t>company</t>
   </si>
   <si>
+    <t>Automation QA Engineer</t>
+  </si>
+  <si>
+    <t>Server QA Engineer for Tango</t>
+  </si>
+  <si>
+    <t>Middle / Senior Automation QA engineer (Python)</t>
+  </si>
+  <si>
+    <t>Senior QA engineer (back-end)</t>
+  </si>
+  <si>
+    <t>Senior QA Engineer</t>
+  </si>
+  <si>
+    <t>Middle / Senior Software Developer in Test (Automation QA Engineer)</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>Software QA Engineer (automation, DevOps)</t>
+  </si>
+  <si>
+    <t>Software Developer In Test (Automation QA Engineer)</t>
+  </si>
+  <si>
+    <t>QA Automation Engineer</t>
+  </si>
+  <si>
+    <t>Solution DevOps/QA Engineer</t>
+  </si>
+  <si>
+    <t>QA Engineer in Automation (Senior / Remote)</t>
+  </si>
+  <si>
+    <t>QA engineer - GTB Liquidity Deposits</t>
+  </si>
+  <si>
     <t>QA engineer (Data + Python)</t>
   </si>
   <si>
-    <t>QA Engineer in Automation (Senior / Remote)</t>
-  </si>
-  <si>
-    <t>QA Automation Engineer</t>
-  </si>
-  <si>
-    <t>QA Engineer</t>
-  </si>
-  <si>
-    <t>Middle / Senior Automation QA engineer (Python)</t>
-  </si>
-  <si>
-    <t>Solution DevOps/QA Engineer</t>
-  </si>
-  <si>
-    <t>Software QA engineer</t>
-  </si>
-  <si>
-    <t>QA Automation Engineer / SDET</t>
-  </si>
-  <si>
-    <t>Software QA Engineer (automation, DevOps)</t>
-  </si>
-  <si>
-    <t>QA Engineer to Backend team (remote)</t>
-  </si>
-  <si>
-    <t>Senior QA engineer (back-end)</t>
-  </si>
-  <si>
-    <t>Senior QA engineer (Senior Software Development Engineer in Test)</t>
-  </si>
-  <si>
-    <t>QA Automation Engineer (Python)</t>
-  </si>
-  <si>
-    <t>Automation QA Engineer</t>
-  </si>
-  <si>
-    <t>Server QA Engineer for Tango</t>
-  </si>
-  <si>
-    <t>QA engineer - GTB Liquidity Deposits</t>
+    <t>Senior QA Performance Tester (Telemedicine Solutions)</t>
   </si>
   <si>
     <t>C++ Gameplay Developer</t>
   </si>
   <si>
-    <t>Software Developer In Test (Automation QA Engineer)</t>
-  </si>
-  <si>
-    <t>Senior QA Engineer</t>
+    <t>QA Engineer (Scanner)</t>
+  </si>
+  <si>
+    <t>Middle DevOps Engineer with AWS Experience (Telehealth Solutions)</t>
   </si>
   <si>
     <t>Remote Automation QA Engineer</t>
   </si>
   <si>
-    <t>Middle / Senior Software Developer in Test (Automation QA Engineer)</t>
-  </si>
-  <si>
     <t>QA Engineer/Инженер по качеству</t>
   </si>
   <si>
@@ -124,66 +118,66 @@
     <t>Senior QA Engineer (remote)</t>
   </si>
   <si>
+    <t>https://samara.hh.ru/vacancy/45464664?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46623115?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/45830450?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/44603951?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46099033?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46289269?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/45537546?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46565978?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46666346?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46279032?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46426583?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/37640164?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46344647?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46664211?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/44407757?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
     <t>https://samara.hh.ru/vacancy/45783106?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/46344647?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46279032?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46514414?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/45830450?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46426583?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46534977?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46485527?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46565978?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/40813843?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/44603951?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46317991?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46002351?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/45464664?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46623115?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46664211?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/45970120?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46666346?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46099033?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+    <t>https://samara.hh.ru/vacancy/46519657?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
     <t>https://samara.hh.ru/vacancy/45970119?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
+    <t>https://samara.hh.ru/vacancy/45384380?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46539920?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
     <t>https://samara.hh.ru/vacancy/46274579?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
@@ -244,172 +238,172 @@
     <t>https://samara.hh.ru/vacancy/41646932?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
     <t>руб.</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>USD</t>
+    <t>3500</t>
   </si>
   <si>
     <t>5000</t>
   </si>
   <si>
-    <t>3500</t>
-  </si>
-  <si>
     <t>200000</t>
   </si>
   <si>
     <t>150000</t>
   </si>
   <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
     <t>250000</t>
   </si>
   <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>300000</t>
-  </si>
-  <si>
-    <t>4000</t>
+    <t>Минск, Молодежная</t>
+  </si>
+  <si>
+    <t>Киев</t>
+  </si>
+  <si>
+    <t>Харьков</t>
+  </si>
+  <si>
+    <t>Минск</t>
+  </si>
+  <si>
+    <t>Минск, Немига</t>
+  </si>
+  <si>
+    <t>Гомель</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург</t>
   </si>
   <si>
     <t>Москва</t>
   </si>
   <si>
-    <t xml:space="preserve">Санкт-Петербург, Василеостровская и еще 1 </t>
-  </si>
-  <si>
-    <t>Харьков</t>
-  </si>
-  <si>
-    <t>Санкт-Петербург</t>
+    <t>Омск</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Москва, Новокузнецкая и еще 2 </t>
+  </si>
+  <si>
+    <t>Гродно</t>
+  </si>
+  <si>
+    <t>Москва, Тульская</t>
+  </si>
+  <si>
+    <t>Херсон</t>
+  </si>
+  <si>
+    <t>Екатеринбург</t>
+  </si>
+  <si>
+    <t>Витебск</t>
+  </si>
+  <si>
+    <t>Нижний Новгород</t>
+  </si>
+  <si>
+    <t>Саратов</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург, Адмиралтейская</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург, Лиговский проспект</t>
+  </si>
+  <si>
+    <t>Алматы</t>
+  </si>
+  <si>
+    <t>Могилев</t>
+  </si>
+  <si>
+    <t>Краснодар</t>
   </si>
   <si>
     <t>Новосибирск</t>
   </si>
   <si>
-    <t>Минск</t>
-  </si>
-  <si>
-    <t>Санкт-Петербург, Горьковская</t>
-  </si>
-  <si>
-    <t>Минск, Молодежная</t>
-  </si>
-  <si>
-    <t>Киев</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Москва, Новокузнецкая и еще 2 </t>
-  </si>
-  <si>
-    <t>Минск, Немига</t>
-  </si>
-  <si>
-    <t>Екатеринбург</t>
-  </si>
-  <si>
-    <t>Витебск</t>
-  </si>
-  <si>
-    <t>Нижний Новгород</t>
-  </si>
-  <si>
-    <t>Саратов</t>
-  </si>
-  <si>
-    <t>Санкт-Петербург, Адмиралтейская</t>
-  </si>
-  <si>
-    <t>Санкт-Петербург, Лиговский проспект</t>
-  </si>
-  <si>
-    <t>Алматы</t>
-  </si>
-  <si>
-    <t>Могилев</t>
-  </si>
-  <si>
-    <t>Краснодар</t>
-  </si>
-  <si>
     <t>Казань</t>
   </si>
   <si>
     <t>Владивосток</t>
   </si>
   <si>
+    <t>ООО Изибрэйн</t>
+  </si>
+  <si>
+    <t>Onseo</t>
+  </si>
+  <si>
+    <t>Dish Ukraine</t>
+  </si>
+  <si>
+    <t>Tango Me</t>
+  </si>
+  <si>
+    <t>ООО Инспекторио Бел</t>
+  </si>
+  <si>
+    <t>Godel Technologies Europe</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>Metapix, Inc</t>
+  </si>
+  <si>
+    <t>Genesys</t>
+  </si>
+  <si>
+    <t>ООО Lineate</t>
+  </si>
+  <si>
+    <t>Cloudification GmbH</t>
+  </si>
+  <si>
+    <t>Deutsche Bank Technology Center</t>
+  </si>
+  <si>
     <t>Exness</t>
   </si>
   <si>
-    <t>Cloudification GmbH</t>
-  </si>
-  <si>
-    <t>Metapix, Inc</t>
-  </si>
-  <si>
-    <t>Nedra - New Digital Resources for Assets</t>
-  </si>
-  <si>
-    <t>Dish Ukraine</t>
-  </si>
-  <si>
-    <t>Genesys</t>
-  </si>
-  <si>
-    <t>Schlumberger Telecommunications and Information Security Systems LLC. Офис</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>Tango Me</t>
-  </si>
-  <si>
-    <t>Fivetran</t>
+    <t>DataArt</t>
+  </si>
+  <si>
+    <t>AWEM</t>
+  </si>
+  <si>
+    <t>Align Technology</t>
+  </si>
+  <si>
+    <t>Scopic Software</t>
+  </si>
+  <si>
+    <t>OS33</t>
+  </si>
+  <si>
+    <t>ООО СолбегСофт</t>
   </si>
   <si>
     <t>Grid Dynamics</t>
   </si>
   <si>
-    <t>ООО Изибрэйн</t>
-  </si>
-  <si>
-    <t>Onseo</t>
-  </si>
-  <si>
-    <t>Deutsche Bank Technology Center</t>
-  </si>
-  <si>
-    <t>AWEM</t>
-  </si>
-  <si>
-    <t>Godel Technologies Europe</t>
-  </si>
-  <si>
-    <t>ООО Инспекторио Бел</t>
-  </si>
-  <si>
-    <t>Scopic Software</t>
-  </si>
-  <si>
-    <t>OS33</t>
-  </si>
-  <si>
-    <t>ООО СолбегСофт</t>
-  </si>
-  <si>
     <t>Itiviti (Айтивити)</t>
-  </si>
-  <si>
-    <t>ООО Lineate</t>
   </si>
   <si>
     <t>Velvetech, LLC</t>
@@ -820,19 +814,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -843,22 +831,13 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -869,22 +848,13 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -895,13 +865,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -912,13 +882,13 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -929,13 +899,13 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -946,13 +916,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -963,19 +933,13 @@
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -986,13 +950,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1003,19 +967,22 @@
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H11" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1026,13 +993,13 @@
         <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1040,22 +1007,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="H13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1063,16 +1024,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1080,16 +1050,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1097,16 +1067,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H16" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1114,16 +1084,22 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" t="s">
+        <v>83</v>
       </c>
       <c r="G17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1131,16 +1107,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1148,16 +1124,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="H19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1165,16 +1141,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1182,16 +1158,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G21" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1199,16 +1175,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1216,16 +1192,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H23" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1233,16 +1209,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1250,16 +1226,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G25" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1267,16 +1243,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H26" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1284,22 +1260,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
         <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1307,16 +1283,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G28" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H28" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1324,22 +1300,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
         <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1347,22 +1323,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1370,22 +1346,22 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F31" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H31" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1393,25 +1369,25 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H32" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1419,16 +1395,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H33" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1436,16 +1412,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1453,16 +1429,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H35" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1470,16 +1446,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G36" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="H36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1487,16 +1463,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1504,16 +1480,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1521,16 +1497,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H39" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1538,16 +1514,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H40" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1555,16 +1531,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H41" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add task 1 Update 4
</commit_message>
<xml_diff>
--- a/vacancy.xlsx
+++ b/vacancy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="132">
   <si>
     <t>name</t>
   </si>
@@ -37,16 +37,58 @@
     <t>company</t>
   </si>
   <si>
+    <t>QA engineer (Data + Python)</t>
+  </si>
+  <si>
+    <t>QA Engineer in Automation (Senior / Remote)</t>
+  </si>
+  <si>
+    <t>QA Automation Engineer</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>Middle / Senior Automation QA engineer (Python)</t>
+  </si>
+  <si>
+    <t>Solution DevOps/QA Engineer</t>
+  </si>
+  <si>
+    <t>Software QA engineer</t>
+  </si>
+  <si>
+    <t>QA Automation Engineer / SDET</t>
+  </si>
+  <si>
+    <t>Software QA Engineer (automation, DevOps)</t>
+  </si>
+  <si>
+    <t>QA Engineer to Backend team (remote)</t>
+  </si>
+  <si>
+    <t>Senior QA engineer (back-end)</t>
+  </si>
+  <si>
+    <t>Senior QA engineer (Senior Software Development Engineer in Test)</t>
+  </si>
+  <si>
+    <t>QA Automation Engineer (Python)</t>
+  </si>
+  <si>
     <t>Automation QA Engineer</t>
   </si>
   <si>
     <t>Server QA Engineer for Tango</t>
   </si>
   <si>
-    <t>Middle / Senior Automation QA engineer (Python)</t>
-  </si>
-  <si>
-    <t>Senior QA engineer (back-end)</t>
+    <t>QA engineer - GTB Liquidity Deposits</t>
+  </si>
+  <si>
+    <t>C++ Gameplay Developer</t>
+  </si>
+  <si>
+    <t>Software Developer In Test (Automation QA Engineer)</t>
   </si>
   <si>
     <t>Senior QA Engineer</t>
@@ -55,144 +97,102 @@
     <t>Middle / Senior Software Developer in Test (Automation QA Engineer)</t>
   </si>
   <si>
-    <t>QA Engineer</t>
-  </si>
-  <si>
-    <t>Software QA Engineer (automation, DevOps)</t>
-  </si>
-  <si>
-    <t>Software Developer In Test (Automation QA Engineer)</t>
-  </si>
-  <si>
-    <t>QA Automation Engineer</t>
-  </si>
-  <si>
-    <t>Solution DevOps/QA Engineer</t>
-  </si>
-  <si>
-    <t>QA Engineer in Automation (Senior / Remote)</t>
-  </si>
-  <si>
-    <t>QA engineer - GTB Liquidity Deposits</t>
-  </si>
-  <si>
-    <t>QA engineer (Data + Python)</t>
-  </si>
-  <si>
-    <t>Senior QA Performance Tester (Telemedicine Solutions)</t>
-  </si>
-  <si>
-    <t>C++ Gameplay Developer</t>
-  </si>
-  <si>
-    <t>QA Engineer (Scanner)</t>
-  </si>
-  <si>
-    <t>Middle DevOps Engineer with AWS Experience (Telehealth Solutions)</t>
-  </si>
-  <si>
-    <t>Remote Automation QA Engineer</t>
-  </si>
-  <si>
     <t>QA Engineer/Инженер по качеству</t>
   </si>
   <si>
+    <t>Golang Developer</t>
+  </si>
+  <si>
     <t>Performance Testing Engineer (Middle / Senior)</t>
   </si>
   <si>
-    <t>Golang Developer</t>
+    <t>Automation QA</t>
   </si>
   <si>
     <t>Automation QA specialist</t>
   </si>
   <si>
-    <t>Automation QA</t>
+    <t>QA Automation Engineer (remote)</t>
   </si>
   <si>
     <t>QA Engineer - тестировщик</t>
   </si>
   <si>
-    <t>QA Automation Engineer (remote)</t>
-  </si>
-  <si>
     <t>Senior QA Engineer (remote)</t>
   </si>
   <si>
+    <t>https://samara.hh.ru/vacancy/45783106?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46344647?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46279032?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46514414?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/45830450?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46426583?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46534977?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46485527?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46565978?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/40813843?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/44603951?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46317991?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46002351?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
     <t>https://samara.hh.ru/vacancy/45464664?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
     <t>https://samara.hh.ru/vacancy/46623115?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/45830450?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/44603951?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+    <t>https://samara.hh.ru/vacancy/46664211?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/45970120?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46666346?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
     <t>https://samara.hh.ru/vacancy/46099033?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/46289269?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/45537546?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46565978?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46666346?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46279032?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46426583?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/37640164?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46344647?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46664211?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/44407757?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/45783106?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46519657?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
     <t>https://samara.hh.ru/vacancy/45970119?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/45384380?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46539920?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46274579?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
     <t>https://samara.hh.ru/vacancy/41773854?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
     <t>https://samara.hh.ru/vacancy/46267962?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
+    <t>https://samara.hh.ru/vacancy/43158201?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
     <t>https://samara.hh.ru/vacancy/46248029?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/43158201?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
     <t>https://samara.hh.ru/vacancy/44240510?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
@@ -202,70 +202,97 @@
     <t>https://samara.hh.ru/vacancy/44181442?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
+    <t>https://samara.hh.ru/vacancy/46089628?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
     <t>https://samara.hh.ru/vacancy/46089629?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/46089628?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+    <t>https://samara.hh.ru/vacancy/46056967?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46066347?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
     <t>https://samara.hh.ru/vacancy/46068040?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/46056967?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+    <t>https://samara.hh.ru/vacancy/46066344?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46066346?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>https://samara.hh.ru/vacancy/46066345?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
     <t>https://samara.hh.ru/vacancy/46066343?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/46066346?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46066344?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46066347?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
-    <t>https://samara.hh.ru/vacancy/46066345?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
     <t>https://samara.hh.ru/vacancy/41646986?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
-    <t>https://samara.hh.ru/vacancy/41646987?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
-  </si>
-  <si>
     <t>https://samara.hh.ru/vacancy/41646932?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
   </si>
   <si>
+    <t>https://samara.hh.ru/vacancy/41646985?from=vacancy_search_result&amp;query=Python%20tester%20new</t>
+  </si>
+  <si>
+    <t>руб.</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
     <t>USD</t>
   </si>
   <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>руб.</t>
+    <t>5000</t>
   </si>
   <si>
     <t>3500</t>
   </si>
   <si>
-    <t>5000</t>
-  </si>
-  <si>
     <t>200000</t>
   </si>
   <si>
     <t>150000</t>
   </si>
   <si>
+    <t>250000</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
     <t>2000</t>
   </si>
   <si>
-    <t>3000</t>
-  </si>
-  <si>
-    <t>250000</t>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Санкт-Петербург, Василеостровская и еще 1 </t>
+  </si>
+  <si>
+    <t>Харьков</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург</t>
+  </si>
+  <si>
+    <t>Новосибирск</t>
+  </si>
+  <si>
+    <t>Минск</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург, Горьковская</t>
   </si>
   <si>
     <t>Минск, Молодежная</t>
@@ -274,73 +301,79 @@
     <t>Киев</t>
   </si>
   <si>
-    <t>Харьков</t>
-  </si>
-  <si>
-    <t>Минск</t>
+    <t xml:space="preserve">Москва, Новокузнецкая и еще 2 </t>
   </si>
   <si>
     <t>Минск, Немига</t>
   </si>
   <si>
-    <t>Гомель</t>
-  </si>
-  <si>
-    <t>Санкт-Петербург</t>
-  </si>
-  <si>
-    <t>Москва</t>
-  </si>
-  <si>
-    <t>Омск</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Москва, Новокузнецкая и еще 2 </t>
-  </si>
-  <si>
-    <t>Гродно</t>
-  </si>
-  <si>
-    <t>Москва, Тульская</t>
-  </si>
-  <si>
-    <t>Херсон</t>
+    <t>Витебск</t>
+  </si>
+  <si>
+    <t>Нижний Новгород</t>
+  </si>
+  <si>
+    <t>Саратов</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург, Адмиралтейская</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург, Лиговский проспект</t>
+  </si>
+  <si>
+    <t>Алматы</t>
+  </si>
+  <si>
+    <t>Могилев</t>
+  </si>
+  <si>
+    <t>Казань</t>
+  </si>
+  <si>
+    <t>Краснодар</t>
+  </si>
+  <si>
+    <t>Владивосток</t>
   </si>
   <si>
     <t>Екатеринбург</t>
   </si>
   <si>
-    <t>Витебск</t>
-  </si>
-  <si>
-    <t>Нижний Новгород</t>
-  </si>
-  <si>
-    <t>Саратов</t>
-  </si>
-  <si>
-    <t>Санкт-Петербург, Адмиралтейская</t>
-  </si>
-  <si>
-    <t>Санкт-Петербург, Лиговский проспект</t>
-  </si>
-  <si>
-    <t>Алматы</t>
-  </si>
-  <si>
-    <t>Могилев</t>
-  </si>
-  <si>
-    <t>Краснодар</t>
-  </si>
-  <si>
-    <t>Новосибирск</t>
-  </si>
-  <si>
-    <t>Казань</t>
-  </si>
-  <si>
-    <t>Владивосток</t>
+    <t>Ростов-на-Дону</t>
+  </si>
+  <si>
+    <t>Exness</t>
+  </si>
+  <si>
+    <t>Cloudification GmbH</t>
+  </si>
+  <si>
+    <t>Metapix, Inc</t>
+  </si>
+  <si>
+    <t>Nedra - New Digital Resources for Assets</t>
+  </si>
+  <si>
+    <t>Dish Ukraine</t>
+  </si>
+  <si>
+    <t>Genesys</t>
+  </si>
+  <si>
+    <t>Schlumberger Telecommunications and Information Security Systems LLC. Офис</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>Tango Me</t>
+  </si>
+  <si>
+    <t>Fivetran</t>
+  </si>
+  <si>
+    <t>Grid Dynamics</t>
   </si>
   <si>
     <t>ООО Изибрэйн</t>
@@ -349,61 +382,31 @@
     <t>Onseo</t>
   </si>
   <si>
-    <t>Dish Ukraine</t>
-  </si>
-  <si>
-    <t>Tango Me</t>
+    <t>Deutsche Bank Technology Center</t>
+  </si>
+  <si>
+    <t>AWEM</t>
+  </si>
+  <si>
+    <t>Godel Technologies Europe</t>
   </si>
   <si>
     <t>ООО Инспекторио Бел</t>
   </si>
   <si>
-    <t>Godel Technologies Europe</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>Metapix, Inc</t>
-  </si>
-  <si>
-    <t>Genesys</t>
+    <t>OS33</t>
+  </si>
+  <si>
+    <t>ООО СолбегСофт</t>
+  </si>
+  <si>
+    <t>Itiviti (Айтивити)</t>
   </si>
   <si>
     <t>ООО Lineate</t>
   </si>
   <si>
-    <t>Cloudification GmbH</t>
-  </si>
-  <si>
-    <t>Deutsche Bank Technology Center</t>
-  </si>
-  <si>
-    <t>Exness</t>
-  </si>
-  <si>
-    <t>DataArt</t>
-  </si>
-  <si>
-    <t>AWEM</t>
-  </si>
-  <si>
-    <t>Align Technology</t>
-  </si>
-  <si>
     <t>Scopic Software</t>
-  </si>
-  <si>
-    <t>OS33</t>
-  </si>
-  <si>
-    <t>ООО СолбегСофт</t>
-  </si>
-  <si>
-    <t>Grid Dynamics</t>
-  </si>
-  <si>
-    <t>Itiviti (Айтивити)</t>
   </si>
   <si>
     <t>Velvetech, LLC</t>
@@ -814,10 +817,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
         <v>109</v>
@@ -831,10 +840,19 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
         <v>110</v>
@@ -848,7 +866,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
+        <v>83</v>
       </c>
       <c r="G4" t="s">
         <v>86</v>
@@ -865,7 +892,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
         <v>87</v>
@@ -882,7 +909,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
         <v>88</v>
@@ -899,7 +926,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
         <v>89</v>
@@ -916,13 +943,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -933,13 +960,19 @@
         <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>84</v>
       </c>
       <c r="G9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -950,13 +983,13 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -967,22 +1000,19 @@
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>74</v>
       </c>
-      <c r="E11" t="s">
-        <v>77</v>
-      </c>
       <c r="F11" t="s">
         <v>81</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -993,10 +1023,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H12" t="s">
         <v>117</v>
@@ -1007,13 +1037,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" t="s">
+        <v>85</v>
       </c>
       <c r="G13" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
         <v>118</v>
@@ -1024,22 +1060,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" t="s">
-        <v>82</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H14" t="s">
         <v>119</v>
@@ -1050,10 +1077,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G15" t="s">
         <v>93</v>
@@ -1067,16 +1094,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G16" t="s">
         <v>94</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1084,22 +1111,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1107,16 +1128,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1124,16 +1145,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G19" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="H19" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1141,16 +1162,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1158,16 +1179,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H21" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1175,16 +1196,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G22" t="s">
         <v>97</v>
       </c>
       <c r="H22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1192,16 +1213,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G23" t="s">
         <v>98</v>
       </c>
       <c r="H23" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1209,16 +1230,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G24" t="s">
         <v>99</v>
       </c>
       <c r="H24" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1226,13 +1247,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H25" t="s">
         <v>127</v>
@@ -1243,10 +1264,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" t="s">
+        <v>79</v>
       </c>
       <c r="G26" t="s">
         <v>100</v>
@@ -1260,16 +1287,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" t="s">
-        <v>76</v>
-      </c>
-      <c r="E27" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
         <v>101</v>
@@ -1283,16 +1304,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E28" t="s">
+        <v>80</v>
       </c>
       <c r="G28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H28" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1300,22 +1327,22 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
         <v>76</v>
       </c>
-      <c r="E29" t="s">
-        <v>80</v>
+      <c r="F29" t="s">
+        <v>83</v>
       </c>
       <c r="G29" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H29" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1323,22 +1350,22 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1346,22 +1373,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="G31" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="H31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1369,25 +1390,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" t="s">
-        <v>77</v>
-      </c>
-      <c r="F32" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="G32" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="H32" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1395,16 +1407,25 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="D33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" t="s">
+        <v>83</v>
       </c>
       <c r="G33" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="H33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1415,13 +1436,13 @@
         <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G34" t="s">
         <v>90</v>
       </c>
       <c r="H34" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1432,13 +1453,13 @@
         <v>32</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G35" t="s">
         <v>105</v>
       </c>
       <c r="H35" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1449,13 +1470,13 @@
         <v>32</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G36" t="s">
         <v>106</v>
       </c>
       <c r="H36" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1466,13 +1487,13 @@
         <v>32</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G37" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H37" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1480,16 +1501,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="G38" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="H38" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1497,16 +1518,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>71</v>
       </c>
       <c r="G39" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H39" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1514,16 +1535,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G40" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H40" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1531,16 +1552,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>73</v>
       </c>
       <c r="G41" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="H41" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>